<commit_message>
Renamed some page object models
</commit_message>
<xml_diff>
--- a/SupportTicket/ExcelData/sample.xlsx
+++ b/SupportTicket/ExcelData/sample.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CreateTicket" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -31,7 +32,69 @@
     <t xml:space="preserve">rajesh.s</t>
   </si>
   <si>
-    <t xml:space="preserve">test@123</t>
+    <t xml:space="preserve">Kays@csg126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assign contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attachment file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helpdesk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Title is to test create another ticket with automation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh.s created this ticket, data set is fetched from excel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajni sandhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajni.s@kaysharbor.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">New image file attached from excel</t>
   </si>
 </sst>
 </file>
@@ -41,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -64,16 +127,61 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF5983B0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -81,6 +189,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -107,9 +222,49 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -121,6 +276,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF5983B0"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -132,36 +347,36 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="test@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="Kays@csg126"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -171,4 +386,170 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="Rajni.s@kaysharbor.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented POM on complete create ticket script.
</commit_message>
<xml_diff>
--- a/SupportTicket/ExcelData/sample.xlsx
+++ b/SupportTicket/ExcelData/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">assign contact</t>
   </si>
   <si>
-    <t xml:space="preserve">Add Cc</t>
+    <t xml:space="preserve"> Cc Email</t>
   </si>
   <si>
     <t xml:space="preserve">Attachment file</t>
@@ -59,10 +59,16 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Helpdesk</t>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineering</t>
   </si>
   <si>
     <t xml:space="preserve"> Title is to test create another ticket with automation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banner bank</t>
   </si>
   <si>
     <t xml:space="preserve">rajesh.s created this ticket, data set is fetched from excel.</t>
@@ -80,6 +86,7 @@
         <color rgb="FF008000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">123</t>
     </r>
@@ -89,12 +96,16 @@
         <color rgb="FF000000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.jpg</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">New image file attached from excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUTH GRANTS</t>
   </si>
 </sst>
 </file>
@@ -140,19 +151,20 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Consolas"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF008000"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -222,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,19 +255,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,7 +298,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000C0"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -346,7 +362,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -393,21 +409,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="43.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +435,7 @@
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -435,110 +453,126 @@
       <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="G2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>